<commit_message>
reran ocl experiments prior failing due to bugs in repair mechanism
</commit_message>
<xml_diff>
--- a/LLM_OCL_experiments/EvaluationData.xlsx
+++ b/LLM_OCL_experiments/EvaluationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Workspace\github\c4s.CQRS-passiveworkflowengine\src\test\resources\oclLlmEval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\workspace\eclipse-workspace\c4s.CQRS-passiveworkflowengine\LLM_OCL_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AC187B-9BF2-4B41-9A0B-0C18CC8F663A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0F1016-45A6-4DC5-9757-D684B4B58402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="2460" windowWidth="25740" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>1a</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Nonexisting Properties/methods</t>
   </si>
   <si>
-    <t>a bit convoluted as it starts from outBugs and outReqs instead of going from req to bugs directly but otherwise structurally correct, uses 'not Closed' as equivalent of 'equals Active' , non-existing method 'belongs to' incorrectly replaced with  isDefined (instead of perhaps better: includes)</t>
-  </si>
-  <si>
     <t>assumes inCRs contain all the requirements' CRs, uses 'markedDeleted' as 'non-released' flag instead of state</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>YNN</t>
   </si>
   <si>
-    <t>initially partially wrong entry element (hence nonexisting property), if all released, then one has review that is not open, does not navigate to findings</t>
-  </si>
-  <si>
     <t>Worsening repair</t>
   </si>
   <si>
@@ -180,54 +174,38 @@
     <t>assumes that all TestCase successors are Reviews, also similar ambiguity as in 1c: ground truth interprets as one test case exists, but all that exist must have […]. LLM interprets at least one TC with […] exists</t>
   </si>
   <si>
-    <t>NNN</t>
-  </si>
-  <si>
-    <t>Failed 3x to extract OCL from flow text</t>
-  </si>
-  <si>
-    <t>YYN</t>
-  </si>
-  <si>
     <t>assumes that Bugs must have a link to Requrement</t>
   </si>
   <si>
-    <t>does not check whether CR is non-released, checks uncessarily that all req issues are children of CR, but otherwise much shorted</t>
-  </si>
-  <si>
     <t xml:space="preserve">check if one TC tests Req instead of all, </t>
   </si>
   <si>
     <t>uses Bug's testCaseItems instead of testedByItems</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Repair used wrong type - fix repair and rerun!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!! Does not check for active issue, otherwise ok</t>
-    </r>
+    <t>does not check whether CR is non-released, checks uncessarily that all req issues are children of CR, but otherwise much shorter</t>
+  </si>
+  <si>
+    <t>Does not check for active issue, otherwise ok</t>
+  </si>
+  <si>
+    <t>incorrect/hallucinated navigate to findings</t>
+  </si>
+  <si>
+    <t>description does not specifiy which property refers to Reviewfindings</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>requires that requirement has bug and that bug has tc that test this bug, would need implies,  and tc tests req</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,13 +216,6 @@
     <font>
       <sz val="11"/>
       <color theme="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -576,27 +547,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.9296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.53125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="5.3984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="5.3984375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="5.1328125" style="4" customWidth="1"/>
-    <col min="9" max="11" width="4.9296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="6.06640625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="5.265625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="73.73046875" customWidth="1"/>
-    <col min="15" max="15" width="33.265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" style="4" customWidth="1"/>
+    <col min="7" max="8" width="5.140625" style="4" customWidth="1"/>
+    <col min="9" max="11" width="5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="6" style="7" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="73.7109375" customWidth="1"/>
+    <col min="15" max="15" width="33.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="122.65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
@@ -604,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>30</v>
@@ -625,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>12</v>
@@ -640,12 +611,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -656,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -677,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="8">
         <v>1</v>
@@ -689,7 +660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -700,7 +671,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -733,7 +704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -744,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -765,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L5" s="8">
         <v>1</v>
@@ -777,7 +748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -788,7 +759,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -824,7 +795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -835,7 +806,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -868,7 +839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -879,7 +850,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -900,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" s="8">
         <v>0.9</v>
@@ -912,21 +883,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="5">
         <v>1</v>
@@ -935,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -947,16 +918,13 @@
         <v>0</v>
       </c>
       <c r="L9" s="8">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -967,7 +935,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -988,24 +956,24 @@
         <v>0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L10" s="8">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="M10" s="4">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>20</v>
@@ -1044,23 +1012,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1090,21 +1058,21 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -1116,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -1134,24 +1102,24 @@
         <v>2</v>
       </c>
       <c r="N15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -1181,27 +1149,27 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -1219,33 +1187,33 @@
         <v>0</v>
       </c>
       <c r="K17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M17" s="4">
         <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -1275,82 +1243,115 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
       </c>
       <c r="L19" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M19" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
       </c>
       <c r="L20" s="8">
         <v>0.9</v>
       </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
       <c r="N20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1380,21 +1381,21 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -1424,10 +1425,10 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first qwen2.5 experiement run, has bugs, needs work in syntax handling of types
</commit_message>
<xml_diff>
--- a/LLM_OCL_experiments/EvaluationData.xlsx
+++ b/LLM_OCL_experiments/EvaluationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\workspace\eclipse-workspace\c4s.CQRS-passiveworkflowengine\LLM_OCL_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0F1016-45A6-4DC5-9757-D684B4B58402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80223772-D3CD-4A59-9EE7-C568F8CFA302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="2460" windowWidth="25740" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="2460" windowWidth="25740" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="57">
   <si>
     <t>1a</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>requires that requirement has bug and that bug has tc that test this bug, would need implies,  and tc tests req</t>
+  </si>
+  <si>
+    <t>Qwen2.5</t>
   </si>
 </sst>
 </file>
@@ -545,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1434,56 @@
         <v>49</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ran additional llm experiemnts
</commit_message>
<xml_diff>
--- a/LLM_OCL_experiments/EvaluationData.xlsx
+++ b/LLM_OCL_experiments/EvaluationData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Workspace\github\c4s.CQRS-passiveworkflowengine\LLM_OCL_experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\workspace\eclipse-workspace\c4s.CQRS-passiveworkflowengine\LLM_OCL_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB142EA7-D4A1-4670-8072-8CC0C4785E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FB1C7E-8918-427F-A24A-28A6A8CB8D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6360" yWindow="3285" windowWidth="25740" windowHeight="18420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
+    <sheet name="CMD" sheetId="1" r:id="rId1"/>
+    <sheet name="Anmol" sheetId="3" r:id="rId2"/>
+    <sheet name="COnstraint" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
   <si>
     <t>1a</t>
   </si>
@@ -63,9 +65,6 @@
     <t>Only OCL returned</t>
   </si>
   <si>
-    <t>Corrected Properties</t>
-  </si>
-  <si>
     <t>Correct semantics</t>
   </si>
   <si>
@@ -81,12 +80,6 @@
     <t>Autocorrected Types</t>
   </si>
   <si>
-    <t>Added Typ Info</t>
-  </si>
-  <si>
-    <t>Corrected Methods</t>
-  </si>
-  <si>
     <t>Initially Correct Syntax</t>
   </si>
   <si>
@@ -244,13 +237,82 @@
   </si>
   <si>
     <t>fix by (1) replace exists with forAll, (2) relace affectsItems with testsItems, (3) add testsItems check for requirements</t>
+  </si>
+  <si>
+    <t>Correct Context used</t>
+  </si>
+  <si>
+    <t>Added Typ Info to make property ok</t>
+  </si>
+  <si>
+    <t>Corrected Properties (renamed)</t>
+  </si>
+  <si>
+    <t>Corrected Methods (renamed)</t>
+  </si>
+  <si>
+    <t>Unnecessary type info</t>
+  </si>
+  <si>
+    <t>Ensure that all bugs trace (via 'affects') to at least one requirement that is not in status 'Released'.</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>Potential Ambiguity</t>
+  </si>
+  <si>
+    <t>Ensure that each Requirement traces (via 'predecessor') only to other Change Requests which are in state 'Released' or have a priority 1 Issue as a child.</t>
+  </si>
+  <si>
+    <t>only change requests as predecessor vs some predecessors are CRs / only issues as child vs some issues in childItems</t>
+  </si>
+  <si>
+    <t>Ensure that each Requirement traces (via 'tested by') to at least one Test Case in state 'Released'.</t>
+  </si>
+  <si>
+    <t>Ensure that all Requirements in state 'released' trace (via 'successor') to at least one Review, all which must not have any 'open' Review Findings.</t>
+  </si>
+  <si>
+    <t>only  reviews as successors vs some successors are reviews / one review exists with cond vs all reviews must have that condition</t>
+  </si>
+  <si>
+    <t>Ensure that each Requirement with priority '1' traces (via 'tested by') to at least one Test Case that in turn has all Reviews (via 'successor')) in state 'closed'.</t>
+  </si>
+  <si>
+    <t>only TC via testedBy vs some are TCs / only reviews via successor vs some successors are Reviews</t>
+  </si>
+  <si>
+    <t>Ensure for each Requirement that is 'affected by' a Bug has at least one of the requirement's 'tested by' Test Cases trace (via 'tests') to this Bug.</t>
+  </si>
+  <si>
+    <t>only Bugs affectedBy / only TC testedBy / BUT NOT TC tests Bugs and Requirements</t>
+  </si>
+  <si>
+    <t>Ensure that either all Bugs for priority '1' 'affects' Requirements are 'Closed' or otherwise that the Requirement is traced (as 'predecessor') from one of the Change Request's 'active' child Issues.</t>
+  </si>
+  <si>
+    <t>Property for 'Closed' REQ / only Issues from CR childIssues, only CR are in Issue's predecessor</t>
+  </si>
+  <si>
+    <t>Ensure all Requirements with a 'successor' trace to an 'active' Issue (if any), need to have that Issue traced as a 'child' from the Requirement's current (non-released) Change Request.</t>
+  </si>
+  <si>
+    <t>what is an active issue, REQ successors only issues, only Issues as child from CR,  what property from REQ to CR</t>
+  </si>
+  <si>
+    <t>Ensure that every Bug's Testcase directly 'tests' at least one of the Requirements 'affected by' the Bug.</t>
+  </si>
+  <si>
+    <t>what property from Bug to TC, TC only test REQs?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +326,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -286,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -309,6 +377,19 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,181 +671,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.59765625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="5.3984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.73046875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="5.3984375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="5.1328125" style="4" customWidth="1"/>
-    <col min="9" max="11" width="5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="6" style="7" customWidth="1"/>
-    <col min="13" max="13" width="5.265625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="73.73046875" customWidth="1"/>
-    <col min="15" max="15" width="13.265625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="29.796875" customWidth="1"/>
+    <col min="3" max="4" width="5.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="5.140625" style="4" customWidth="1"/>
+    <col min="10" max="13" width="5" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="73.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="8">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -781,40 +867,41 @@
       <c r="J5" s="5">
         <v>0</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="8">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
@@ -828,40 +915,41 @@
       <c r="K6" s="5">
         <v>0</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
         <v>0.8</v>
       </c>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
@@ -875,31 +963,32 @@
       <c r="K7" s="5">
         <v>0</v>
       </c>
-      <c r="L7" s="8">
-        <v>1</v>
-      </c>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -916,75 +1005,77 @@
       <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="8">
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="8">
         <v>0.9</v>
       </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
       <c r="G9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
         <v>3</v>
       </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
       <c r="J9" s="5">
         <v>0</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
       </c>
-      <c r="L9" s="8">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -1001,181 +1092,183 @@
       <c r="J10" s="5">
         <v>0</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="8">
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="8">
         <v>0.8</v>
       </c>
-      <c r="M10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
       </c>
       <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
       <c r="I11" s="5">
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
         <v>0.8</v>
       </c>
-      <c r="M11" s="4">
+      <c r="O11" s="4">
         <v>3</v>
       </c>
-      <c r="N11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2</v>
+      </c>
+      <c r="P15" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>1</v>
-      </c>
-      <c r="M14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>3</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="8">
-        <v>1</v>
-      </c>
-      <c r="M15" s="4">
-        <v>2</v>
-      </c>
-      <c r="N15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="Q15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
@@ -1188,43 +1281,43 @@
       <c r="K16" s="4">
         <v>0</v>
       </c>
-      <c r="L16" s="8">
-        <v>1</v>
-      </c>
       <c r="M16" s="4">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4">
+        <v>30</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4">
         <v>3</v>
       </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
@@ -1235,43 +1328,43 @@
       <c r="K17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
         <v>0.9</v>
       </c>
-      <c r="M17" s="4">
+      <c r="O17" s="4">
         <v>3</v>
       </c>
-      <c r="N17" t="s">
-        <v>51</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
         <v>3</v>
       </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
       <c r="H18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="4">
         <v>0</v>
@@ -1280,43 +1373,43 @@
         <v>0</v>
       </c>
       <c r="K18" s="4">
-        <v>1</v>
-      </c>
-      <c r="L18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="4">
         <v>1</v>
       </c>
-      <c r="N18" t="s">
-        <v>44</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N18" s="8">
+        <v>1</v>
+      </c>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
         <v>2</v>
       </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
       <c r="H19" s="4">
         <v>0</v>
       </c>
@@ -1329,40 +1422,40 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="8">
         <v>0.8</v>
       </c>
-      <c r="M19" s="4">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
         <v>3</v>
       </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
       <c r="H20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -1373,41 +1466,41 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="8">
         <v>0.9</v>
       </c>
-      <c r="M20" s="4">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
-        <v>50</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O20" s="4">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
         <v>3</v>
       </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
       <c r="H21" s="4">
         <v>0</v>
       </c>
@@ -1415,43 +1508,43 @@
         <v>0</v>
       </c>
       <c r="J21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="8">
         <v>0.8</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O21" s="4">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="4">
-        <v>0</v>
-      </c>
       <c r="H22" s="4">
         <v>0</v>
       </c>
@@ -1464,46 +1557,46 @@
       <c r="K22" s="4">
         <v>0</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="8">
         <v>0.9</v>
       </c>
-      <c r="M22" s="4">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>47</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O22" s="4">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
       <c r="H25" s="4">
         <v>0</v>
       </c>
@@ -1516,40 +1609,40 @@
       <c r="K25" s="4">
         <v>0</v>
       </c>
-      <c r="L25" s="7">
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+      <c r="N25" s="7">
         <v>100</v>
       </c>
-      <c r="M25" s="4">
-        <v>1</v>
-      </c>
-      <c r="N25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O25" s="4">
+        <v>1</v>
+      </c>
+      <c r="P25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
         <v>3</v>
       </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
       <c r="H26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1560,38 +1653,38 @@
       <c r="K26" s="4">
         <v>0</v>
       </c>
-      <c r="L26" s="7">
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
         <v>100</v>
       </c>
-      <c r="M26" s="4">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O26" s="4">
+        <v>1</v>
+      </c>
+      <c r="P26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="4">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
         <v>2</v>
       </c>
-      <c r="G27" s="4">
-        <v>0</v>
-      </c>
       <c r="H27" s="4">
         <v>0</v>
       </c>
@@ -1604,38 +1697,38 @@
       <c r="K27" s="4">
         <v>0</v>
       </c>
-      <c r="L27" s="7">
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="7">
         <v>100</v>
       </c>
-      <c r="M27" s="4">
+      <c r="O27" s="4">
         <v>2</v>
       </c>
-      <c r="N27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
         <v>2</v>
       </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
       <c r="H28" s="4">
         <v>0</v>
       </c>
@@ -1648,46 +1741,46 @@
       <c r="K28" s="4">
         <v>0</v>
       </c>
-      <c r="L28" s="7">
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
         <v>90</v>
       </c>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
-      <c r="N28" t="s">
-        <v>58</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>52</v>
+      <c r="O28" s="4">
+        <v>1</v>
       </c>
       <c r="P28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F29" s="4">
         <v>0</v>
       </c>
       <c r="G29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="4">
         <v>0</v>
@@ -1698,87 +1791,87 @@
       <c r="K29" s="4">
         <v>0</v>
       </c>
-      <c r="L29" s="7">
+      <c r="M29" s="4">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
         <v>100</v>
       </c>
-      <c r="M29" s="4">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O29" s="4">
+        <v>1</v>
+      </c>
+      <c r="P29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="4">
+        <v>30</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="4">
         <v>2</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
         <v>5</v>
       </c>
-      <c r="G30" s="4">
-        <v>1</v>
-      </c>
       <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="I30" s="4">
-        <v>0</v>
-      </c>
       <c r="J30" s="4">
         <v>0</v>
       </c>
       <c r="K30" s="4">
-        <v>1</v>
-      </c>
-      <c r="L30" s="7">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1</v>
+      </c>
+      <c r="N30" s="7">
         <v>50</v>
       </c>
-      <c r="M30" s="4">
+      <c r="O30" s="4">
         <v>3</v>
       </c>
-      <c r="N30" t="s">
-        <v>60</v>
-      </c>
       <c r="P30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="R30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
         <v>4</v>
       </c>
-      <c r="G31" s="4">
-        <v>1</v>
-      </c>
       <c r="H31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
@@ -1789,41 +1882,41 @@
       <c r="K31" s="4">
         <v>0</v>
       </c>
-      <c r="L31" s="7">
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
         <v>80</v>
       </c>
-      <c r="M31" s="4">
+      <c r="O31" s="4">
         <v>2</v>
       </c>
-      <c r="N31" t="s">
-        <v>63</v>
-      </c>
       <c r="P31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="R31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
         <v>3</v>
       </c>
-      <c r="G32" s="4">
-        <v>0</v>
-      </c>
       <c r="H32" s="4">
         <v>0</v>
       </c>
@@ -1831,46 +1924,46 @@
         <v>0</v>
       </c>
       <c r="J32" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="4">
-        <v>0</v>
-      </c>
-      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
         <v>60</v>
       </c>
-      <c r="M32" s="4">
-        <v>1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>66</v>
+      <c r="O32" s="4">
+        <v>1</v>
       </c>
       <c r="P32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="R32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
         <v>3</v>
       </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
       <c r="H33" s="4">
         <v>0</v>
       </c>
@@ -1883,21 +1976,159 @@
       <c r="K33" s="4">
         <v>0</v>
       </c>
-      <c r="L33" s="7">
+      <c r="M33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7">
         <v>70</v>
       </c>
-      <c r="M33" s="4">
-        <v>1</v>
-      </c>
-      <c r="N33" t="s">
-        <v>69</v>
+      <c r="O33" s="4">
+        <v>1</v>
       </c>
       <c r="P33" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="R33" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6448EA-1173-4010-BFFE-B0AF28461C29}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64D191F-AD9A-43BC-9964-0B8DD8DE7E54}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="107.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>